<commit_message>
[PERFECTIVE] Removed Parameterizable from Firmness selections (refs #66).
</commit_message>
<xml_diff>
--- a/doc/extensions/kactus2Parameters.xlsx
+++ b/doc/extensions/kactus2Parameters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="23820" windowHeight="14445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
   <si>
     <t>Design aspect</t>
   </si>
@@ -87,9 +87,6 @@
     <t>SYS</t>
   </si>
   <si>
-    <t>Parameterizable</t>
-  </si>
-  <si>
     <t>Mapping</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>KTS_MUTABLE</t>
   </si>
   <si>
-    <t>KTS_PARAMETERIZABLE</t>
-  </si>
-  <si>
     <t>KTS_FIXED</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
   </si>
   <si>
     <t>Component can be  fully configured</t>
-  </si>
-  <si>
-    <t>Component can be parametrized</t>
   </si>
   <si>
     <t>Component can not be configured in any way, it is frozen</t>
@@ -246,8 +237,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +718,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -805,6 +801,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -839,6 +836,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1014,14 +1012,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
@@ -1030,51 +1028,51 @@
     <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" thickBot="1">
+    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>26</v>
-      </c>
       <c r="E1" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1082,68 +1080,68 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
@@ -1151,42 +1149,42 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
@@ -1194,391 +1192,367 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="11"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E14" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="13"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="11"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A18" s="36"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="34"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="35"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="24" spans="1:5" ht="19.5" thickBot="1">
-      <c r="A24" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="25"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="10"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="26"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="11"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="26"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>54</v>
-      </c>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="1"/>
       <c r="C28" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="26"/>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="11"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="29" t="s">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="26"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="26"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="26"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="11"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="26"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="26"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="30" t="s">
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="26"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="13"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="26"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="11"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="26"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="13"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="28" t="s">
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>59</v>
-      </c>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="11"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="29" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="26"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="30" t="s">
+      <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="26"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="34"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A44" s="35"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="35"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="30" t="s">
         <v>70</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1588,24 +1562,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>